<commit_message>
Test modification on Excel
</commit_message>
<xml_diff>
--- a/Project3TestPlan.xlsx
+++ b/Project3TestPlan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickshute/Library/Mobile Documents/com~apple~CloudDocs/School/Winter 2022/CIS 436/Projects/Project 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickshute/AndroidStudioProjects/CIS436P3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BA21ACC-F821-FC40-87B5-F73F65DA2940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C54391-65EC-6646-8146-83485FEA3CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>#</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Not yet implemented</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -575,7 +578,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -661,6 +664,9 @@
       <c r="E4" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="F4" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="G4" s="6" t="s">
         <v>8</v>
       </c>
@@ -687,6 +693,9 @@
       <c r="E5" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="F5" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="G5" s="6" t="s">
         <v>8</v>
       </c>
@@ -713,6 +722,9 @@
       <c r="E6" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="F6" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="G6" s="6" t="s">
         <v>8</v>
       </c>
@@ -739,6 +751,9 @@
       <c r="E7" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="F7" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="G7" s="6" t="s">
         <v>8</v>
       </c>
@@ -764,6 +779,9 @@
       </c>
       <c r="E8" s="2" t="s">
         <v>26</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Added a UI to place all of our API call
</commit_message>
<xml_diff>
--- a/Project3TestPlan.xlsx
+++ b/Project3TestPlan.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickshute/AndroidStudioProjects/CIS436P3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C54391-65EC-6646-8146-83485FEA3CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F64924-D3ED-5343-8CF5-1232FAD910AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Apr 10 2022" sheetId="1" r:id="rId1"/>
+    <sheet name="Apr 14 2022" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -578,7 +578,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -608,7 +608,7 @@
     </row>
     <row r="2" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
-        <v>44661</v>
+        <v>44665</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>

</xml_diff>

<commit_message>
Fixed bottom fragment to be a Scroll View. Also added description and updated test plan
</commit_message>
<xml_diff>
--- a/Project3TestPlan.xlsx
+++ b/Project3TestPlan.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickshute/AndroidStudioProjects/CIS436P3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F64924-D3ED-5343-8CF5-1232FAD910AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8BFE2B-AE38-7D4D-98A4-45B314EA0CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Apr 14 2022" sheetId="1" r:id="rId1"/>
+    <sheet name="Apr 16 2022" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>#</t>
   </si>
@@ -112,13 +112,19 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Nick</t>
+  </si>
+  <si>
+    <t>Passed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,8 +165,14 @@
       <name val="Arial Black"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +193,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -233,7 +251,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -263,6 +281,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -578,7 +599,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -608,7 +629,7 @@
     </row>
     <row r="2" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
-        <v>44665</v>
+        <v>44667</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -661,20 +682,17 @@
       <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>8</v>
+        <v>28</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added names to README.md and updated testplan
</commit_message>
<xml_diff>
--- a/Project3TestPlan.xlsx
+++ b/Project3TestPlan.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickshute/AndroidStudioProjects/CIS436P3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8BFE2B-AE38-7D4D-98A4-45B314EA0CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE08FA05-DB03-D14E-8C27-30964FF834A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apr 16 2022" sheetId="1" r:id="rId1"/>
+    <sheet name="Apr 19 2022" sheetId="2" r:id="rId2"/>
+    <sheet name="Apr 20 2022" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="1" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="2" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="30">
   <si>
     <t>#</t>
   </si>
@@ -271,6 +275,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -281,9 +288,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -598,7 +602,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -615,30 +619,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="A2" s="10">
         <v>44667</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -685,13 +689,507 @@
       <c r="F4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" s="3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1145496-5089-5443-9940-A2192FF65027}">
+  <dimension ref="A1:I28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="35.5" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
+    <col min="7" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+    </row>
+    <row r="2" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>44670</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" s="3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3501852-05FC-D744-ABD9-48FF37FFD461}">
+  <dimension ref="A1:I28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="35.5" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
+    <col min="7" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+    </row>
+    <row r="2" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>44671</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Added names to README.md and updated testplan"
This reverts commit 65912c2d2c629c915ec85df96b7b77efeed7eecd.
</commit_message>
<xml_diff>
--- a/Project3TestPlan.xlsx
+++ b/Project3TestPlan.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickshute/AndroidStudioProjects/CIS436P3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE08FA05-DB03-D14E-8C27-30964FF834A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8BFE2B-AE38-7D4D-98A4-45B314EA0CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apr 16 2022" sheetId="1" r:id="rId1"/>
-    <sheet name="Apr 19 2022" sheetId="2" r:id="rId2"/>
-    <sheet name="Apr 20 2022" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="1" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="2" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -32,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>#</t>
   </si>
@@ -275,9 +271,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -288,6 +281,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -602,7 +598,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -619,30 +615,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="9">
         <v>44667</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -689,507 +685,13 @@
       <c r="F4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" s="3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1145496-5089-5443-9940-A2192FF65027}">
-  <dimension ref="A1:I28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" customWidth="1"/>
-    <col min="4" max="4" width="35.5" customWidth="1"/>
-    <col min="5" max="5" width="28.1640625" customWidth="1"/>
-    <col min="6" max="6" width="19.5" customWidth="1"/>
-    <col min="7" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-    </row>
-    <row r="2" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <v>44670</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" s="3" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3501852-05FC-D744-ABD9-48FF37FFD461}">
-  <dimension ref="A1:I28"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" customWidth="1"/>
-    <col min="4" max="4" width="35.5" customWidth="1"/>
-    <col min="5" max="5" width="28.1640625" customWidth="1"/>
-    <col min="6" max="6" width="19.5" customWidth="1"/>
-    <col min="7" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-    </row>
-    <row r="2" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <v>44671</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="11" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>